<commit_message>
CAmbio de dolares manual 2 cambio del excel
</commit_message>
<xml_diff>
--- a/public/excels/tipoCambios.xlsx
+++ b/public/excels/tipoCambios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\construction\public\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54780DAF-6E09-408C-BB4C-C5227FAB3F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A19985B-EED6-4D30-A96D-DD05E2105894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E71981C3-ACD0-4811-9523-441FD37F6C40}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -74,7 +74,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -389,10 +389,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2A6E81-359E-415E-A94C-0B058B1FA3C8}">
-  <dimension ref="A1:C601"/>
+  <dimension ref="A1:C605"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A589" workbookViewId="0">
+      <selection activeCell="B606" sqref="B606"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7011,6 +7011,50 @@
         <v>3.746</v>
       </c>
     </row>
+    <row r="602" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A602" s="1">
+        <v>45436</v>
+      </c>
+      <c r="B602">
+        <v>3.73</v>
+      </c>
+      <c r="C602">
+        <v>3.7389999999999999</v>
+      </c>
+    </row>
+    <row r="603" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A603" s="1">
+        <v>45437</v>
+      </c>
+      <c r="B603">
+        <v>3.73</v>
+      </c>
+      <c r="C603">
+        <v>3.7389999999999999</v>
+      </c>
+    </row>
+    <row r="604" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A604" s="1">
+        <v>45438</v>
+      </c>
+      <c r="B604">
+        <v>3.73</v>
+      </c>
+      <c r="C604">
+        <v>3.7389999999999999</v>
+      </c>
+    </row>
+    <row r="605" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A605" s="1">
+        <v>45439</v>
+      </c>
+      <c r="B605">
+        <v>3.73</v>
+      </c>
+      <c r="C605">
+        <v>3.7389999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>